<commit_message>
Added CD298 as cell boundary marker
</commit_message>
<xml_diff>
--- a/phenocycler/latest/phenocycler.xlsx
+++ b/phenocycler/latest/phenocycler.xlsx
@@ -232,7 +232,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="246">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -933,6 +933,9 @@
     <t>NAKATPASE</t>
   </si>
   <si>
+    <t>CD298</t>
+  </si>
+  <si>
     <t>nuclear_marker_or_stain</t>
   </si>
   <si>
@@ -960,7 +963,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-01-09T09:33:24-08:00</t>
+    <t>2024-01-09T10:03:04-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1165,13 +1168,13 @@
         <v>230</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2">
@@ -1179,7 +1182,7 @@
         <v>64</v>
       </c>
       <c r="Z2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -1237,7 +1240,7 @@
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'cell_boundary_marker_or_stain'!$A$1:$A$2</formula1>
+      <formula1>'cell_boundary_marker_or_stain'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'nuclear_marker_or_stain'!$A$1:$A$2</formula1>
@@ -1251,7 +1254,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1265,6 +1268,11 @@
     <row r="2">
       <c r="A2" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1287,7 +1295,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -1311,16 +1319,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2">
@@ -1328,13 +1336,13 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new acquisition vendor and models
</commit_message>
<xml_diff>
--- a/phenocycler/latest/phenocycler.xlsx
+++ b/phenocycler/latest/phenocycler.xlsx
@@ -232,7 +232,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="266">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -525,6 +525,18 @@
     <t>acquisition_instrument_vendor</t>
   </si>
   <si>
+    <t>In-House</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
+  </si>
+  <si>
+    <t>BGI Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024848</t>
+  </si>
+  <si>
     <t>Resolve Biosciences</t>
   </si>
   <si>
@@ -567,6 +579,12 @@
     <t>https://identifiers.org/RRID:SCR_017365</t>
   </si>
   <si>
+    <t>Akoya Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023774</t>
+  </si>
+  <si>
     <t>Evident Scientific (Olympus)</t>
   </si>
   <si>
@@ -609,6 +627,12 @@
     <t>https://identifiers.org/RRID:SCR_010233</t>
   </si>
   <si>
+    <t>Motic</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024856</t>
+  </si>
+  <si>
     <t>Ionpath</t>
   </si>
   <si>
@@ -642,6 +666,12 @@
     <t>https://identifiers.org/RRID:SCR_023760</t>
   </si>
   <si>
+    <t>MoticEasyScan One</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024855</t>
+  </si>
+  <si>
     <t>Axio Observer 7</t>
   </si>
   <si>
@@ -660,18 +690,42 @@
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>DM6 B</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024857</t>
+  </si>
+  <si>
     <t>NanoZoomer 2.0-HT</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_021658</t>
   </si>
   <si>
+    <t>Phenocycler-Fusion 2.0</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023773</t>
+  </si>
+  <si>
     <t>Lightsheet 7</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_024448</t>
   </si>
   <si>
+    <t>Phenocycler-Fusion 1.0</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024847</t>
+  </si>
+  <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
   </si>
   <si>
@@ -762,6 +816,12 @@
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
+    <t>Custom: Multiphoton</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
+  </si>
+  <si>
     <t>QTRAP 5500</t>
   </si>
   <si>
@@ -963,7 +1023,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-01-09T12:04:17-08:00</t>
+    <t>2024-01-18T09:31:07-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1120,61 +1180,61 @@
         <v>96</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>237</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2">
@@ -1182,7 +1242,7 @@
         <v>64</v>
       </c>
       <c r="Z2" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -1197,10 +1257,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$15</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$39</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$45</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1262,17 +1322,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -1290,12 +1350,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -1319,16 +1379,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="C1" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="D1" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2">
@@ -1336,13 +1396,13 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="D2" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -1753,7 +1813,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1879,6 +1939,38 @@
         <v>126</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1886,7 +1978,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1894,314 +1986,362 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B22" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B23" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B24" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B25" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B26" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B27" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B28" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B29" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B30" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B31" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B32" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B33" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B34" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B35" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B36" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B37" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B38" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B39" t="s">
-        <v>205</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>214</v>
+      </c>
+      <c r="B40" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>218</v>
+      </c>
+      <c r="B42" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>220</v>
+      </c>
+      <c r="B43" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>222</v>
+      </c>
+      <c r="B44" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>224</v>
+      </c>
+      <c r="B45" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2219,42 +2359,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2272,26 +2412,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="B1" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2309,18 +2449,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "Pan-Cytokeratin,Collagen IV,FUT4,SMA" as an option for the cell boundary stain
</commit_message>
<xml_diff>
--- a/phenocycler/latest/phenocycler.xlsx
+++ b/phenocycler/latest/phenocycler.xlsx
@@ -233,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="350">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1246,6 +1246,9 @@
     <t>CD298</t>
   </si>
   <si>
+    <t>Pan-Cytokeratin,Collagen IV,FUT4,SMA</t>
+  </si>
+  <si>
     <t>nuclear_marker_or_stain</t>
   </si>
   <si>
@@ -1273,7 +1276,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-05-12T10:14:11-07:00</t>
+    <t>2025-05-21T11:20:00-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1478,13 +1481,13 @@
         <v>334</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2">
@@ -1492,7 +1495,7 @@
         <v>76</v>
       </c>
       <c r="Z2" t="s" s="27">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -1550,7 +1553,7 @@
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'cell_boundary_marker_or_stain'!$A$1:$A$3</formula1>
+      <formula1>'cell_boundary_marker_or_stain'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'nuclear_marker_or_stain'!$A$1:$A$2</formula1>
@@ -1564,7 +1567,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1582,6 +1585,11 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>182</v>
       </c>
     </row>
@@ -1600,7 +1608,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2">
@@ -1629,16 +1637,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2">
@@ -1646,13 +1654,13 @@
         <v>76</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new instrument vendor and model
Closes #94
</commit_message>
<xml_diff>
--- a/phenocycler/latest/phenocycler.xlsx
+++ b/phenocycler/latest/phenocycler.xlsx
@@ -231,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="354">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -296,7 +296,7 @@
     <t>Stereo-seq</t>
   </si>
   <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000434</t>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
   </si>
   <si>
     <t>Visium (with probes)</t>
@@ -638,6 +638,12 @@
     <t>https://identifiers.org/RRID:SCR_027007</t>
   </si>
   <si>
+    <t>3DHISTECH</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027042</t>
+  </si>
+  <si>
     <t>GE Healthcare</t>
   </si>
   <si>
@@ -791,6 +797,12 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>Pannoramic MIDI II Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024834</t>
+  </si>
+  <si>
     <t>Not applicable</t>
   </si>
   <si>
@@ -1274,7 +1286,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-06-04T13:59:43-07:00</t>
+    <t>2025-06-10T14:10:14-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1431,61 +1443,61 @@
         <v>124</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2">
@@ -1493,7 +1505,7 @@
         <v>78</v>
       </c>
       <c r="Z2" t="s" s="27">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -1508,10 +1520,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$27</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$28</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$69</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1573,16 +1585,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2">
@@ -1590,13 +1602,13 @@
         <v>78</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -2119,7 +2131,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2341,6 +2353,14 @@
         <v>178</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>179</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2348,7 +2368,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2356,546 +2376,554 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>153</v>
+        <v>298</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>154</v>
+        <v>299</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>296</v>
+        <v>155</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>297</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>316</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2913,42 +2941,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -2966,26 +2994,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -3003,18 +3031,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>